<commit_message>
fiks A ipk 4
</commit_message>
<xml_diff>
--- a/bin/data.xlsx
+++ b/bin/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20705" windowHeight="8185" activeTab="5"/>
+    <workbookView windowWidth="20705" windowHeight="7457" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="admin" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>id_admin</t>
   </si>
@@ -52,18 +52,6 @@
     <t>alamat</t>
   </si>
   <si>
-    <t>UserTest</t>
-  </si>
-  <si>
-    <t>user@com</t>
-  </si>
-  <si>
-    <t>ee11cbb19052e40b07aac0ca060c23ee</t>
-  </si>
-  <si>
-    <t>JOGJA</t>
-  </si>
-  <si>
     <t>id_antrean</t>
   </si>
   <si>
@@ -79,118 +67,13 @@
     <t>jadwal(sore)</t>
   </si>
   <si>
-    <t>21/06/2022_SORE_1</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>SORE</t>
-  </si>
-  <si>
     <t>jadwal</t>
   </si>
   <si>
-    <t>21/06/2022_SORE_2</t>
-  </si>
-  <si>
-    <t>21/06/2022_SORE_3</t>
-  </si>
-  <si>
-    <t>21/06/2022_SORE_4</t>
-  </si>
-  <si>
-    <t>21/06/2022_SORE_5</t>
-  </si>
-  <si>
-    <t>21/06/2022_PAGI_1</t>
-  </si>
-  <si>
-    <t>PAGI</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>next</t>
-  </si>
-  <si>
-    <t>baru</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>demo</t>
-  </si>
-  <si>
-    <t>demo@com</t>
-  </si>
-  <si>
-    <t>fe01ce2a7fbac8fafaed7c982a04e229</t>
-  </si>
-  <si>
-    <t>3_PASIEN</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>098f6bcd4621d373cade4e832627b4f6</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>4_PASIEN</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>5_PASIEN</t>
-  </si>
-  <si>
-    <t>bisa</t>
-  </si>
-  <si>
-    <t>bisa@com</t>
-  </si>
-  <si>
-    <t>8cfff3c034ab00b49315b4f37507230d</t>
-  </si>
-  <si>
-    <t>1_PASIEN</t>
-  </si>
-  <si>
-    <t>22/06/2022_PAGI_1</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>22/06/2022_PAGI_2</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
 </sst>
 </file>
@@ -200,8 +83,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -239,9 +122,31 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,6 +156,36 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -262,26 +197,41 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -292,38 +242,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -336,44 +257,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -390,19 +273,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,7 +435,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,151 +453,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -581,6 +464,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -596,8 +494,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -632,6 +530,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -657,169 +564,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1158,7 +1041,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.15" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1221,7 +1104,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.15" outlineLevelCol="4"/>
   <cols>
     <col min="2" max="2" customWidth="true" width="19.0"/>
     <col min="3" max="3" customWidth="true" width="14.7132352941176"/>
@@ -1257,7 +1140,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D12"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.15" outlineLevelCol="6"/>
@@ -1271,16 +1154,16 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -1298,26 +1181,29 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.15" outlineLevelCol="3"/>
   <cols>
-    <col min="4" max="4" customWidth="true" width="12.3676470588235"/>
+    <col min="1" max="1" customWidth="true" width="17.6029411764706"/>
+    <col min="2" max="2" customWidth="true" width="14.375"/>
+    <col min="3" max="3" customWidth="true" width="14.9264705882353"/>
+    <col min="4" max="4" customWidth="true" width="14.1544117647059"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1218,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:D6"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.15" outlineLevelCol="3"/>
@@ -1344,16 +1230,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1375,10 +1261,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>